<commit_message>
Changes made in Plotting
</commit_message>
<xml_diff>
--- a/truss_analysis.xlsx
+++ b/truss_analysis.xlsx
@@ -44,27 +44,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -92,24 +77,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -477,10 +468,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -492,8 +483,8 @@
     <col width="12.77734375" customWidth="1" style="1" min="5" max="5"/>
     <col width="8.88671875" customWidth="1" style="1" min="6" max="8"/>
     <col width="11.88671875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="8.88671875" customWidth="1" style="1" min="10" max="13"/>
-    <col width="8.88671875" customWidth="1" style="1" min="14" max="16384"/>
+    <col width="8.88671875" customWidth="1" style="1" min="10" max="14"/>
+    <col width="8.88671875" customWidth="1" style="1" min="15" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -504,240 +495,487 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Node</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>-6</v>
+      <c r="B4" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ELEMENTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Element</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>StartNode</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>EndNode</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>ELEMENTS</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Element</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>StartNode</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>EndNode</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Area</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+      <c r="B21" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="6" t="n"/>
+      <c r="E24" s="7" t="n"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="6" t="n"/>
+      <c r="E25" s="7" t="n"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="6" t="n"/>
+      <c r="E26" s="7" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>LOADS</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>Node</t>
+        </is>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>Fx</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>Fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>-500000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>-200000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>SUPPORTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>Node</t>
+        </is>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Xfixed</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>Yfixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B36" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C36" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="2" t="n">
+      <c r="B37" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>500</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>LOADS</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Node</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>Fx</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Fy</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>100000</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>-200000</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>SUPPORTS</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Node</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>Xfixed</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>Yfixed</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2" t="n">
+      <c r="C42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -752,7 +990,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -761,17 +999,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Node</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>X-Displacement (m)</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Y-Displacement (m)</t>
         </is>
@@ -793,10 +1031,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>-0.06694920972016018</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.012</v>
+        <v>-0.05974837557971645</v>
       </c>
     </row>
     <row r="4">
@@ -804,9 +1042,53 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.005710533733521293</v>
+        <v>0.03965512664157637</v>
       </c>
       <c r="C4" t="n">
+        <v>-0.2754745793920796</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.03147144295437398</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.323859438199801</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.01101187684126581</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.2594661905705234</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.09763166517838652</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.05665346697091067</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -821,7 +1103,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -830,22 +1112,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="inlineStr">
+      <c r="A1" s="8" t="inlineStr">
         <is>
           <t>Element</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Force (N)</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>Stress (Pa)</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>Nature</t>
         </is>
@@ -856,14 +1138,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>200000</v>
+        <v>-481759.3018145688</v>
       </c>
       <c r="C2" t="n">
-        <v>400</v>
+        <v>-963.5186036291375</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tension</t>
+          <t>Compression</t>
         </is>
       </c>
     </row>
@@ -872,14 +1154,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>43927.1825655484</v>
+        <v>-545609.3372531328</v>
       </c>
       <c r="C3" t="n">
-        <v>87.8543651310968</v>
+        <v>-1091.218674506266</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tension</t>
+          <t>Compression</t>
         </is>
       </c>
     </row>
@@ -888,14 +1170,142 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>63450.37481690326</v>
+        <v>-282842.712474619</v>
       </c>
       <c r="C4" t="n">
-        <v>126.9007496338065</v>
+        <v>-565.6854249492379</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Compression</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-424264.0687119286</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-848.5281374238571</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Compression</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-580964.6763124602</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1161.929352624921</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Compression</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-561882.6634915462</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1123.765326983092</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Compression</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>147955.2753891987</v>
+      </c>
+      <c r="C8" t="n">
+        <v>295.9105507783975</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>89953.57256191788</v>
+      </c>
+      <c r="C9" t="n">
+        <v>179.9071451238358</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>34165.44469347098</v>
+      </c>
+      <c r="C10" t="n">
+        <v>68.33088938694196</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Tension</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-44891.49681073849</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-89.78299362147699</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Compression</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-143216.2490015528</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-286.4324980031056</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Compression</t>
         </is>
       </c>
     </row>

</xml_diff>